<commit_message>
first-pass code and figures
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaths\GitHub\covid-data-comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B3AA257-F218-4062-9298-B7F7F2ED7DAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0574900F-81CC-4E03-A121-5AB7062D2AED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7990" yWindow="440" windowWidth="10260" windowHeight="7810" activeTab="1" xr2:uid="{B9D764F1-712F-41F6-AC8C-76E51C061C17}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="4" xr2:uid="{B9D764F1-712F-41F6-AC8C-76E51C061C17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId3"/>
+    <sheet name="ecdc-sources" sheetId="7" r:id="rId4"/>
+    <sheet name="jhu-sources" sheetId="4" r:id="rId5"/>
+    <sheet name="health" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet5" sheetId="9" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">health!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'jhu-sources'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet6!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="212">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -187,6 +197,9 @@
     <t>Cases</t>
   </si>
   <si>
+    <t>Deaths</t>
+  </si>
+  <si>
     <t>Healthcare</t>
   </si>
   <si>
@@ -247,9 +260,6 @@
     <t>Hospitalised</t>
   </si>
   <si>
-    <t>Back-distributed</t>
-  </si>
-  <si>
     <t>https://covid19.who.int/who-data/vaccination-data.csv</t>
   </si>
   <si>
@@ -271,17 +281,413 @@
     <t>Corrections public</t>
   </si>
   <si>
-    <t>Unclear</t>
-  </si>
-  <si>
     <t>Corrections</t>
+  </si>
+  <si>
+    <t>JHU source; no healthcare data</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Weekly</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Czechia</t>
+  </si>
+  <si>
+    <t>JHU weekly effect</t>
+  </si>
+  <si>
+    <t>Out of phase</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>JHU spike</t>
+  </si>
+  <si>
+    <t>JHU zero, ECDC missing</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>JHU negative</t>
+  </si>
+  <si>
+    <t>ECDC truncation</t>
+  </si>
+  <si>
+    <t>Daily cases</t>
+  </si>
+  <si>
+    <t>Daily deaths</t>
+  </si>
+  <si>
+    <t>ECDC spike</t>
+  </si>
+  <si>
+    <t>Italy Ministry of Health</t>
+  </si>
+  <si>
+    <t>Government of Ireland</t>
+  </si>
+  <si>
+    <t>Dati COVID-19 Italia (Italy)</t>
+  </si>
+  <si>
+    <t>Czechia Ministry of Health</t>
+  </si>
+  <si>
+    <t>French Government</t>
+  </si>
+  <si>
+    <t>OpenCOVID19 France</t>
+  </si>
+  <si>
+    <t>National Institute of Health of Kosovo</t>
+  </si>
+  <si>
+    <t>Berliner Morgenpost (Germany)</t>
+  </si>
+  <si>
+    <t>rtve (Spain)</t>
+  </si>
+  <si>
+    <t>Ministry of Health, Republic of Serbia</t>
+  </si>
+  <si>
+    <t>Belgium Sciensano</t>
+  </si>
+  <si>
+    <t>Public Health Agency of Sweden</t>
+  </si>
+  <si>
+    <t>The UK Government</t>
+  </si>
+  <si>
+    <t>Netherlands National Institute for Health and Environment</t>
+  </si>
+  <si>
+    <t>Iceland Directorate of Health and Department of Civil Protection and Emergency Management</t>
+  </si>
+  <si>
+    <t>Luxembourg Government</t>
+  </si>
+  <si>
+    <t>Republic of Turkey Ministry of Health</t>
+  </si>
+  <si>
+    <t>Slovakia Ministry of Investment, Regional Development and Information</t>
+  </si>
+  <si>
+    <t>http://www.salute.gov.it/nuovocoronavirus</t>
+  </si>
+  <si>
+    <t>https://covid19ireland-geohive.hub.arcgis.com/</t>
+  </si>
+  <si>
+    <t>https://github.com/pcm-dpc/COVID-19/tree/master/dati-regioni</t>
+  </si>
+  <si>
+    <t>https://onemocneni-aktualne.mzcr.cz/covid-19</t>
+  </si>
+  <si>
+    <t>https://dashboard.covid19.data.gouv.fr/ and https://www.data.gouv.fr/en/datasets/donnees-relatives-a-lepidemie-de-covid-19-en-france-vue-densemble/</t>
+  </si>
+  <si>
+    <t>https://github.com/opencovid19-fr</t>
+  </si>
+  <si>
+    <t>https://corona-ks.info/?lang=en and https://raw.githubusercontent.com/bgeVam/Kosovo-Coronatracker-Data/master/data.json</t>
+  </si>
+  <si>
+    <t>https://interaktiv.morgenpost.de/corona-virus-karte-infektionen-deutschland-weltweit/</t>
+  </si>
+  <si>
+    <t>https://www.rtve.es/noticias/20200514/mapa-del-coronavirus-espana/2004681.shtml</t>
+  </si>
+  <si>
+    <t>https://covid19.rs/homepage-english/</t>
+  </si>
+  <si>
+    <t>https://datastudio.google.com/embed/reporting/c14a5cfc-cab7-4812-848c-0369173148ab/page/giyUB</t>
+  </si>
+  <si>
+    <t>https://experience.arcgis.com/experience/09f821667ce64bf7be6f9f87457ed9aa</t>
+  </si>
+  <si>
+    <t>https://osp.maps.arcgis.com/apps/MapSeries/index.html?appid=c6bc9659a00449239eb3bde062d23caa</t>
+  </si>
+  <si>
+    <t>https://coronavirus.data.gov.uk/#category=nations&amp;map=rate</t>
+  </si>
+  <si>
+    <t>https://experience.arcgis.com/experience/ea064047519040469acb8da05c0f100d</t>
+  </si>
+  <si>
+    <t>https://www.covid.is/data</t>
+  </si>
+  <si>
+    <t>https://data.public.lu/fr/datasets/covid-19-rapports-journaliers/#_</t>
+  </si>
+  <si>
+    <t>https://covid19.saglik.gov.tr/EN-69532/general-coronavirus-table.html</t>
+  </si>
+  <si>
+    <t>https://korona.gov.sk/</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Lichtenstein</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>issue</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>TESSy</t>
+  </si>
+  <si>
+    <t>JRC + TESSy - https://worldhealthorg.shinyapps.io/euro-covid19/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Austria </t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latvia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liechtenstein </t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source </t>
+  </si>
+  <si>
+    <t>https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+  </si>
+  <si>
+    <t>https://epistat.wiv-isp.be/covid/covid-19.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://covid19.lanix.org/ </t>
+  </si>
+  <si>
+    <t>https://www.koronavirus.hr/zupanije/139</t>
+  </si>
+  <si>
+    <t>https://covid19.ucy.ac.cy/</t>
+  </si>
+  <si>
+    <t>https://www.ssi.dk/sygdomme-beredskab-og-forskning/sygdomsovervaagning/c/covid19-overvaagning</t>
+  </si>
+  <si>
+    <t>https://www.terviseamet.ee/et/koroonaviirus/koroonakaart</t>
+  </si>
+  <si>
+    <t>https://experience.arcgis.com/experience/d40b2aaf08be4b9c8ec38de30b714f26</t>
+  </si>
+  <si>
+    <t>https://experience.arcgis.com/experience/478220a4c454480e823b17327b2bf1d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://covid19.gov.gr/covid19-live-analytics/ </t>
+  </si>
+  <si>
+    <t>https://koronavirus.gov.hu/terkepek/fertozottek</t>
+  </si>
+  <si>
+    <t>https://www.covid.is/tolulegar-upplysingar</t>
+  </si>
+  <si>
+    <t>https://www.gov.ie/en/news/7e0924-latest-updates-on-covid-19-coronavirus/%20and%20go%20into%20the%20section:%20Press%20release%20and%20county-by-county%20figures</t>
+  </si>
+  <si>
+    <t>https://www.arcgis.com/apps/opsdashboard/index.html#/b0c68bce2cce478eaac82fe38d4138b1</t>
+  </si>
+  <si>
+    <t>https://data.gov.lv/dati/lv/dataset/covid-19-pa-adm-terit/resource/492931dd-0012-46d7-b415-76fe0ec7c216</t>
+  </si>
+  <si>
+    <t>https://www.regierung.li/coronavirus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://gouvernement.lu/fr/dossiers.gouv_msan+fr+dossiers+2020+corona-virus.html </t>
+  </si>
+  <si>
+    <t>https://deputyprimeminister.gov.mt/en/health-promotion/Pages/Novel-coronavirus.aspx</t>
+  </si>
+  <si>
+    <t>https://data.rivm.nl/covid-19/</t>
+  </si>
+  <si>
+    <t>https://www.fhi.no/en/id/infectious-diseases/coronavirus/daily-reports/daily-reports-COVID19/</t>
+  </si>
+  <si>
+    <t>https://www.gov.pl/web/koronawirus/wykaz-zarazen-koronawirusem-sars-cov-2</t>
+  </si>
+  <si>
+    <t>https://covid19.min-saude.pt/ponto-de-situacao-atual-em-portugal/</t>
+  </si>
+  <si>
+    <t>https://instnsp.maps.arcgis.com/apps/opsdashboard/index.html#/5eced796595b4ee585bcdba03e30c127</t>
+  </si>
+  <si>
+    <t>https://korona.gov.sk/koronavirus-na-slovensku-v-cislach/</t>
+  </si>
+  <si>
+    <t>https://www.nijz.si/sl/dnevno-spremljanje-okuzb-s-sars-cov-2-covid-19</t>
+  </si>
+  <si>
+    <t>https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/situacionActual.htm</t>
+  </si>
+  <si>
+    <t>https://experience.arcgis.com/experience/2dc63e26f509468f896ec69476b0dab3</t>
+  </si>
+  <si>
+    <t>inc_hosp</t>
+  </si>
+  <si>
+    <t>inc_icu</t>
+  </si>
+  <si>
+    <t>prev_hosp</t>
+  </si>
+  <si>
+    <t>prev_icu</t>
+  </si>
+  <si>
+    <t>prev_respirator</t>
+  </si>
+  <si>
+    <t>Prevalence</t>
+  </si>
+  <si>
+    <t>Incidence</t>
+  </si>
+  <si>
+    <t>ICU</t>
+  </si>
+  <si>
+    <t>Country coverage</t>
+  </si>
+  <si>
+    <t>ECDC - private</t>
+  </si>
+  <si>
+    <t>ECDC - public</t>
+  </si>
+  <si>
+    <t>% data across all date-location combinations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +707,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -327,10 +748,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -648,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E55B14B-A17A-4501-90B4-364974FC4E99}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D8"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -936,10 +1371,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D17DEF8-24C3-4639-A8C2-F487C6FDA6F9}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -948,17 +1383,17 @@
     <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.90625" customWidth="1"/>
     <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
         <v>47</v>
@@ -966,20 +1401,20 @@
       <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
-        <v>55</v>
+      <c r="E1" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
         <v>60</v>
-      </c>
-      <c r="I1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -987,7 +1422,7 @@
         <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -998,7 +1433,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
@@ -1006,44 +1441,47 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="D4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>156</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>45</v>
@@ -1054,7 +1492,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
@@ -1063,21 +1501,21 @@
         <v>48</v>
       </c>
       <c r="H7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" t="s">
-        <v>56</v>
+        <v>64</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="I8" t="s">
         <v>71</v>
@@ -1096,76 +1534,76 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
         <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
         <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" t="s">
         <v>66</v>
-      </c>
-      <c r="I11" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
         <v>48</v>
       </c>
-      <c r="E12" t="s">
-        <v>68</v>
+      <c r="E12" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>155</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" t="s">
         <v>66</v>
       </c>
-      <c r="I12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>46</v>
       </c>
@@ -1173,7 +1611,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>21</v>
       </c>
@@ -1181,7 +1619,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>20</v>
       </c>
@@ -1189,21 +1627,2122 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F25" s="4"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="D37" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I10" r:id="rId1" xr:uid="{987A6E55-D832-4D17-8A25-4F5FCBBFC6FE}"/>
+    <hyperlink ref="I4" r:id="rId2" xr:uid="{ED354CA5-5847-41FE-B02B-516E1A5BE147}"/>
+    <hyperlink ref="H8" r:id="rId3" xr:uid="{53627740-85B7-4F6E-AB10-114ACD513ED4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA2E9B6-B563-466E-AD8E-F6DE8487BE39}">
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" t="s">
+        <v>140</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" t="s">
+        <v>165</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" t="s">
+        <v>166</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" t="s">
+        <v>167</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>145</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" t="s">
+        <v>148</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" t="s">
+        <v>170</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>139</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>149</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>148</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{C1B5ECB6-42DF-43C4-9DA7-11BEA86D4870}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C42">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:D33">
+    <sortCondition ref="D2:D33"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D73732A-F158-499A-8054-94BDA2EB98FC}">
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B53F0A-F3E0-4103-99F8-6BCEDC9539F2}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="61.36328125" style="5" customWidth="1"/>
+    <col min="2" max="16384" width="8.7265625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{37E0390E-2D8D-419B-8D5E-D84630DEE99A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C20">
+      <sortCondition ref="C1"/>
+    </sortState>
+  </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{D7DEB1EA-CD9F-4A90-BC2B-73F1A1F1444D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E80B7B9-1E12-4623-BA66-0C7238B6FCBC}">
+  <dimension ref="A1:T33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9:R14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2">
+        <v>732</v>
+      </c>
+      <c r="E2">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>365</v>
+      </c>
+      <c r="D3">
+        <v>728</v>
+      </c>
+      <c r="E3">
+        <v>728</v>
+      </c>
+      <c r="F3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4">
+        <v>714</v>
+      </c>
+      <c r="E4">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5">
+        <v>327</v>
+      </c>
+      <c r="C5">
+        <v>327</v>
+      </c>
+      <c r="D5">
+        <v>683</v>
+      </c>
+      <c r="E5">
+        <v>714</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6">
+        <v>250</v>
+      </c>
+      <c r="C6">
+        <v>170</v>
+      </c>
+      <c r="D6">
+        <v>737</v>
+      </c>
+      <c r="E6">
+        <v>737</v>
+      </c>
+      <c r="J6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7">
+        <v>420</v>
+      </c>
+      <c r="C7">
+        <v>420</v>
+      </c>
+      <c r="D7">
+        <v>379</v>
+      </c>
+      <c r="E7">
+        <v>379</v>
+      </c>
+      <c r="H7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8">
+        <v>383</v>
+      </c>
+      <c r="D8">
+        <v>565</v>
+      </c>
+      <c r="E8">
+        <v>564</v>
+      </c>
+      <c r="F8">
+        <v>296</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9">
+        <v>386</v>
+      </c>
+      <c r="C9">
+        <v>315</v>
+      </c>
+      <c r="D9">
+        <v>773</v>
+      </c>
+      <c r="E9">
+        <v>770</v>
+      </c>
+      <c r="F9">
+        <v>330</v>
+      </c>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10">
+        <v>597</v>
+      </c>
+      <c r="E10">
+        <v>598</v>
+      </c>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>361</v>
+      </c>
+      <c r="C11">
+        <v>361</v>
+      </c>
+      <c r="D11">
+        <v>790</v>
+      </c>
+      <c r="E11">
+        <v>788</v>
+      </c>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>433</v>
+      </c>
+      <c r="D12">
+        <v>399</v>
+      </c>
+      <c r="E12">
+        <v>720</v>
+      </c>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13">
+        <v>300</v>
+      </c>
+      <c r="C13">
+        <v>280</v>
+      </c>
+      <c r="D13">
+        <v>440</v>
+      </c>
+      <c r="E13">
+        <v>819</v>
+      </c>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D14">
+        <v>720</v>
+      </c>
+      <c r="E14">
+        <v>719</v>
+      </c>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15">
+        <v>169</v>
+      </c>
+      <c r="D15">
+        <v>731</v>
+      </c>
+      <c r="E15">
+        <v>673</v>
+      </c>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16">
+        <v>416</v>
+      </c>
+      <c r="C16">
+        <v>365</v>
+      </c>
+      <c r="D16">
+        <v>774</v>
+      </c>
+      <c r="E16">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>796</v>
+      </c>
+      <c r="E17">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18">
+        <v>427</v>
+      </c>
+      <c r="C18">
+        <v>427</v>
+      </c>
+      <c r="D18">
+        <v>712</v>
+      </c>
+      <c r="E18">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D19">
+        <v>806</v>
+      </c>
+      <c r="E19">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>270</v>
+      </c>
+      <c r="C20">
+        <v>147</v>
+      </c>
+      <c r="D20">
+        <v>523</v>
+      </c>
+      <c r="E20">
+        <v>490</v>
+      </c>
+      <c r="F20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21">
+        <v>724</v>
+      </c>
+      <c r="E21">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22">
+        <v>374</v>
+      </c>
+      <c r="C22">
+        <v>317</v>
+      </c>
+      <c r="D22">
+        <v>458</v>
+      </c>
+      <c r="E22">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23">
+        <v>420</v>
+      </c>
+      <c r="C23">
+        <v>383</v>
+      </c>
+      <c r="D23">
+        <v>773</v>
+      </c>
+      <c r="E23">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24">
+        <v>386</v>
+      </c>
+      <c r="C24">
+        <v>385</v>
+      </c>
+      <c r="D24">
+        <v>595</v>
+      </c>
+      <c r="E24">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25">
+        <v>401</v>
+      </c>
+      <c r="D25">
+        <v>696</v>
+      </c>
+      <c r="E25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>166</v>
+      </c>
+      <c r="B26">
+        <v>416</v>
+      </c>
+      <c r="D26">
+        <v>750</v>
+      </c>
+      <c r="E26">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27">
+        <v>315</v>
+      </c>
+      <c r="D27">
+        <v>371</v>
+      </c>
+      <c r="E27">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28">
+        <v>314</v>
+      </c>
+      <c r="C28">
+        <v>151</v>
+      </c>
+      <c r="D28">
+        <v>710</v>
+      </c>
+      <c r="E28">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29">
+        <v>414</v>
+      </c>
+      <c r="C29">
+        <v>371</v>
+      </c>
+      <c r="D29">
+        <v>760</v>
+      </c>
+      <c r="E29">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30">
+        <v>436</v>
+      </c>
+      <c r="C30">
+        <v>436</v>
+      </c>
+      <c r="D30">
+        <v>424</v>
+      </c>
+      <c r="E30">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31">
+        <v>406</v>
+      </c>
+      <c r="D31">
+        <v>651</v>
+      </c>
+      <c r="E31">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>148</v>
+      </c>
+      <c r="D32">
+        <v>818</v>
+      </c>
+      <c r="E32">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33">
+        <v>377</v>
+      </c>
+      <c r="D33">
+        <v>733</v>
+      </c>
+      <c r="E33">
+        <v>728</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{A221621E-FA44-4E6E-85D9-ABDDD08E6C2F}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7B145A-9AF2-452A-8E12-C1BA4AEF349D}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="10"/>
+      <c r="B1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="10">
+        <v>51</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>47</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" s="10">
+        <v>65</v>
+      </c>
+      <c r="C4" s="10">
+        <v>58</v>
+      </c>
+      <c r="D4" s="10">
+        <v>68</v>
+      </c>
+      <c r="E4" s="10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" s="10">
+        <v>76</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>63</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:E5">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>